<commit_message>
imagine cup entry push
</commit_message>
<xml_diff>
--- a/pagegen/data.xlsx
+++ b/pagegen/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3EC5E8-B3F0-46F6-A31E-67F67EA1CA99}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DB3924-073D-4CC5-ABB7-80992320ABA8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
   <si>
     <t>Title</t>
   </si>
@@ -251,6 +251,27 @@
   </si>
   <si>
     <t>Best Paper of the Special Track on Novel Applications (ICAPS 2013)</t>
+  </si>
+  <si>
+    <t>Projection-Aware Planning</t>
+  </si>
+  <si>
+    <t>Projection-Aware Task Planning and Execution for Human-in-the-Loop Operation of Robots in a Mixed-Reality Workspace</t>
+  </si>
+  <si>
+    <t>Tathagata Chakraborti, Sarath Sreedharan, Anagha Kulkarni and Subbarao Kambhampati</t>
+  </si>
+  <si>
+    <t>Recent advances in mixed-reality technologies have renewed interest in alternative modes of communication for human-robot interaction. However, most of the work in this direction has been confined to tasks such as teleoperation, simulation or explication of individual actions of a robot. In this paper, we will discuss how the capability to project intentions affect the task planning capabilities of a robot. Specifically, we will start with a discussion on how projection actions can be used to reveal information regarding the future intentions of the robot at the time of task execution. We will then pose a new planning paradigm – projection-aware planning – whereby a robot can trade off its plan cost with its ability to reveal its intentions using its projection actions. We demonstrate each of these scenarios with the help of a joint human-robot activity using the HoloLens.</t>
+  </si>
+  <si>
+    <t>U.S. Finals, Microsoft Imagine Cup 2017 (ICAPS Demo Track 2017)</t>
+  </si>
+  <si>
+    <t>imagine</t>
+  </si>
+  <si>
+    <t>http://ae-robots.com/,https://yochan-lab.github.io/papers/files/papers/projection-aware.pdf</t>
   </si>
 </sst>
 </file>
@@ -585,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCF7FF2-5513-4694-9A44-0590350F5772}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -597,6 +618,7 @@
     <col min="2" max="2" width="15.59765625" customWidth="1"/>
     <col min="3" max="3" width="20.06640625" customWidth="1"/>
     <col min="4" max="4" width="18.46484375" customWidth="1"/>
+    <col min="6" max="6" width="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -670,176 +692,200 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{2EC7D9DD-663B-4801-860E-C30C3AFE1AC3}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{2EC7D9DD-663B-4801-860E-C30C3AFE1AC3}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{1F4BFC0B-29EA-455C-B342-671F1801B96B}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{941AFC2A-3037-4343-A90C-3687656B64F6}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{0C53371C-1542-47B8-8D62-04768F1C1D9E}"/>
-    <hyperlink ref="F8" r:id="rId5" xr:uid="{2A0AE6E4-E29F-48D9-863E-04289D662D66}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{A30D5C9D-71A4-46BA-9068-0238955DA6CA}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{A6543A23-C272-4B24-B23F-574A18590A5F}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{0C53371C-1542-47B8-8D62-04768F1C1D9E}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{2A0AE6E4-E29F-48D9-863E-04289D662D66}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{A30D5C9D-71A4-46BA-9068-0238955DA6CA}"/>
+    <hyperlink ref="F11" r:id="rId7" xr:uid="{A6543A23-C272-4B24-B23F-574A18590A5F}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{617F927E-1CCB-4BEB-9DF3-DEF58DB1FEA9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>